<commit_message>
Working script, added new unfinished script
</commit_message>
<xml_diff>
--- a/List.xlsx
+++ b/List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\0 - WORK\CARDANO\Other Projects\For ThisCrazy\BITCOIN\4Fre5hBTC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABB9C38-152D-46DF-97A7-DF762A3FFF15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC62785-4C24-4992-95AD-21DD1F8A4978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v1" sheetId="1" r:id="rId1"/>
@@ -362,15 +362,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="A2:C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" customWidth="1"/>
-    <col min="2" max="2" width="30.77734375" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -403,12 +405,13 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="A2" sqref="A2:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -440,13 +443,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView topLeftCell="A74" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G82" sqref="A2:G82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -479,7 +483,86 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="A2" sqref="A2:F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="19.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,80 +593,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>